<commit_message>
Small change in planning
Changed the week in wich Jip is going to do a spellcheck for the the
research report
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -122,9 +122,6 @@
     <t xml:space="preserve">Onderzoek doen </t>
   </si>
   <si>
-    <t>Onderzoeksrapport nakijken</t>
-  </si>
-  <si>
     <t>Totaal uren per activiteit</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Uitloop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onderzoeksrapport nakijken en klaar maken voor inleveren </t>
   </si>
 </sst>
 </file>
@@ -436,30 +436,6 @@
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -473,12 +449,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -516,6 +486,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,981 +846,979 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="12" t="s">
+      <c r="J1" s="43"/>
+      <c r="K1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="36"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="7"/>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="40">
+      <c r="F3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C4">
         <v>0.5</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="7"/>
       <c r="E4">
         <v>0.5</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="7"/>
       <c r="G4">
         <v>0.5</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="23">
+      <c r="H4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="13">
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="7"/>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="23">
+      <c r="F5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="7"/>
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="7"/>
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="23">
+      <c r="J6" s="7"/>
+      <c r="K6" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="23">
+      <c r="H7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8">
         <v>2</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23">
+      <c r="J8" s="7"/>
+      <c r="K8" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="7"/>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="7"/>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" s="15"/>
+      <c r="H9" s="7"/>
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="23">
+      <c r="J9" s="7"/>
+      <c r="K9" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="25">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15"/>
+      <c r="C10" s="15">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="25">
-        <v>1</v>
-      </c>
-      <c r="H10" s="15"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7"/>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="23">
+      <c r="J10" s="7"/>
+      <c r="K10" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="25">
+      <c r="D11" s="7"/>
+      <c r="E11" s="15">
         <v>10</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="25">
+      <c r="F11" s="7"/>
+      <c r="G11" s="15">
         <v>10</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="28">
+      <c r="H11" s="7"/>
+      <c r="I11" s="18">
         <v>10</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="37">
+      <c r="J11" s="19"/>
+      <c r="K11" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="27">
+      <c r="D12" s="7"/>
+      <c r="E12" s="17">
         <v>10</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="7"/>
       <c r="G12">
         <v>10</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="7"/>
       <c r="I12">
         <v>10</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="23">
+      <c r="J12" s="7"/>
+      <c r="K12" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="25">
+      <c r="C13" s="15"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="15">
         <v>0.5</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="23">
+      <c r="H13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="17">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="27">
-        <v>4</v>
-      </c>
-      <c r="F14" s="15"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="17">
+        <v>4</v>
+      </c>
+      <c r="F14" s="7"/>
       <c r="G14">
         <v>6</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="7"/>
       <c r="I14">
         <v>2</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="23">
+      <c r="J14" s="7"/>
+      <c r="K14" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="27">
-        <v>4</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="27">
-        <v>4</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="C15" s="17">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="17">
+        <v>4</v>
+      </c>
+      <c r="F15" s="7"/>
       <c r="G15">
         <v>4</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="7"/>
       <c r="I15">
         <v>2</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="23">
+      <c r="J15" s="7"/>
+      <c r="K15" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="27">
-        <v>1</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="27">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15"/>
+      <c r="C16" s="17">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7"/>
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="7"/>
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="23">
+      <c r="J16" s="7"/>
+      <c r="K16" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="27">
-        <v>2</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="27">
-        <v>2</v>
-      </c>
-      <c r="F17" s="15"/>
+      <c r="C17" s="17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7"/>
       <c r="G17">
         <v>2</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="7"/>
       <c r="I17">
         <v>2</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="23">
+      <c r="J17" s="7"/>
+      <c r="K17" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="25">
-        <v>2</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="27">
-        <v>2</v>
-      </c>
-      <c r="F18" s="15"/>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="17">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7"/>
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="H18" s="15"/>
+      <c r="H18" s="7"/>
       <c r="I18">
         <v>2</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="23">
+      <c r="J18" s="7"/>
+      <c r="K18" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="15">
         <v>1.5</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="25">
+      <c r="D19" s="2"/>
+      <c r="E19" s="15">
         <v>1.5</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="7"/>
       <c r="G19">
         <v>1.5</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="7"/>
       <c r="I19">
         <v>1.5</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="23">
+      <c r="J19" s="7"/>
+      <c r="K19" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="22">
         <v>40</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32">
+      <c r="D20" s="21"/>
+      <c r="E20" s="22">
         <v>41</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32">
+      <c r="F20" s="21"/>
+      <c r="G20" s="22">
         <v>42</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="32">
+      <c r="H20" s="21"/>
+      <c r="I20" s="22">
         <v>35.5</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="41">
+      <c r="J20" s="20"/>
+      <c r="K20" s="31">
         <v>161</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="8" t="s">
+      <c r="D21" s="37"/>
+      <c r="E21" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="10"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="14" t="s">
+      <c r="G22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="14" t="s">
+      <c r="I22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="36"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="15"/>
+      <c r="D23" s="7"/>
       <c r="E23">
         <v>2</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="28">
-        <v>4</v>
-      </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="37">
+      <c r="F23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="18">
+        <v>4</v>
+      </c>
+      <c r="J23" s="19"/>
+      <c r="K23" s="27">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="7"/>
       <c r="E24">
         <v>10</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="7"/>
       <c r="G24">
         <v>10</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="7"/>
       <c r="I24">
         <v>10</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="23">
+      <c r="J24" s="7"/>
+      <c r="K24" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="21" t="s">
-        <v>41</v>
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="7"/>
       <c r="E25">
         <v>7</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="7"/>
       <c r="G25">
         <v>7</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="7"/>
       <c r="I25">
         <v>7</v>
       </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="23">
+      <c r="J25" s="7"/>
+      <c r="K25" s="13">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="7"/>
       <c r="E26">
         <v>4</v>
       </c>
-      <c r="F26" s="15"/>
+      <c r="F26" s="7"/>
       <c r="G26">
         <v>4</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="7"/>
       <c r="I26">
         <v>4</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="23">
+      <c r="J26" s="7"/>
+      <c r="K26" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="7"/>
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="F27" s="7"/>
+      <c r="H27" s="7"/>
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
-      <c r="B28" s="30" t="s">
+      <c r="J27" s="7"/>
+      <c r="K27" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="23"/>
+      <c r="B29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="31">
+      <c r="C29" s="21">
+        <v>26</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21">
         <v>24</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31">
-        <v>24</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31">
+      <c r="F29" s="20"/>
+      <c r="G29" s="21">
         <v>21</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31">
+      <c r="H29" s="20"/>
+      <c r="I29" s="21">
         <v>26</v>
       </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="38">
+      <c r="J29" s="20"/>
+      <c r="K29" s="28">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="23">
-        <v>2</v>
-      </c>
-    </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="15"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="7"/>
       <c r="E30">
         <v>3</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="25">
+      <c r="F30" s="7"/>
+      <c r="G30" s="15">
         <v>3</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="7"/>
       <c r="I30">
         <v>3</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="23">
+      <c r="J30" s="7"/>
+      <c r="K30" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
-      <c r="B31" s="21" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="17">
+        <v>3</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="J31" s="19"/>
+      <c r="K31" s="27">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="17">
+        <v>3</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="17">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="17">
+        <v>3</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="32">
+        <v>3</v>
+      </c>
+      <c r="J32" s="7"/>
+      <c r="K32" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="15">
+        <v>2</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="15">
+        <v>2</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="15">
+        <v>2</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="32">
+        <v>2</v>
+      </c>
+      <c r="J33" s="7"/>
+      <c r="K33" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="27">
-        <v>3</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="37">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="27">
-        <v>3</v>
-      </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="27">
-        <v>3</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="27">
-        <v>3</v>
-      </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="42">
-        <v>3</v>
-      </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="25">
-        <v>2</v>
-      </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="25">
-        <v>2</v>
-      </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="25">
-        <v>2</v>
-      </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="42">
-        <v>2</v>
-      </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="21" t="s">
+      <c r="C34" s="17">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="17">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="27">
-        <v>1</v>
-      </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="27">
-        <v>1</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="25">
+      <c r="C35" s="15"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="15">
         <v>2.5</v>
       </c>
-      <c r="H35" s="15"/>
+      <c r="H35" s="7"/>
       <c r="I35">
         <v>2.5</v>
       </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="23">
+      <c r="J35" s="7"/>
+      <c r="K35" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="27">
-        <v>1</v>
-      </c>
-      <c r="D36" s="15"/>
-      <c r="E36" s="27">
-        <v>1</v>
-      </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="27">
-        <v>1</v>
-      </c>
-      <c r="H36" s="15"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="17">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="17">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="17">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7"/>
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="J36" s="15"/>
-      <c r="K36" s="23">
+      <c r="J36" s="7"/>
+      <c r="K36" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="21" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="17">
+        <v>2</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="17">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="17">
+        <v>2</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="27">
-        <v>2</v>
-      </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="27">
-        <v>2</v>
-      </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="27">
-        <v>2</v>
-      </c>
-      <c r="H37" s="15"/>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37" s="15"/>
-      <c r="K37" s="23"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="25">
+      <c r="C38" s="15">
         <v>6</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="27">
+      <c r="D38" s="7"/>
+      <c r="E38" s="17">
         <v>6</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="27">
+      <c r="F38" s="7"/>
+      <c r="G38" s="17">
         <v>6</v>
       </c>
-      <c r="H38" s="15"/>
+      <c r="H38" s="7"/>
       <c r="I38">
         <v>6</v>
       </c>
-      <c r="J38" s="15"/>
-      <c r="K38" s="23">
+      <c r="J38" s="7"/>
+      <c r="K38" s="13">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="23"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="43"/>
-      <c r="B40" s="44" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="35">
+        <v>18</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="35">
+        <v>18.5</v>
+      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="35">
         <v>20</v>
       </c>
-      <c r="D40" s="44"/>
-      <c r="E40" s="45">
-        <v>18.5</v>
-      </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="45">
+      <c r="H40" s="34"/>
+      <c r="I40" s="35">
         <v>20</v>
       </c>
-      <c r="H40" s="44"/>
-      <c r="I40" s="45">
-        <v>20</v>
-      </c>
-      <c r="J40" s="43"/>
-      <c r="K40" s="41">
+      <c r="J40" s="33"/>
+      <c r="K40" s="31">
         <v>70.5</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="44">
+      <c r="C42" s="34">
         <v>84</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44">
+      <c r="D42" s="34"/>
+      <c r="E42" s="34">
         <v>83.5</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44">
+      <c r="F42" s="34"/>
+      <c r="G42" s="34">
         <v>83</v>
       </c>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44">
+      <c r="H42" s="34"/>
+      <c r="I42" s="34">
         <v>81.5</v>
       </c>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44">
+      <c r="J42" s="34"/>
+      <c r="K42" s="34">
         <v>332</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited object list  and added autosom to planning
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Jip</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Van takenlijst een concurrecy diagram maken</t>
   </si>
   <si>
-    <t>Klasse maken voor speakertje</t>
-  </si>
-  <si>
-    <t>Klasse maken voor keypad</t>
-  </si>
-  <si>
     <t>Rtos libary doccumentatie bekijken</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Rtos functionaliteiten integreren in klassen</t>
   </si>
   <si>
-    <t xml:space="preserve">overgebleven klasse schrijven uit het klassediagram </t>
-  </si>
-  <si>
     <t>Onderzoeksverslag nakijken</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>Code checken volgens regels</t>
   </si>
   <si>
-    <t>overgebleven klasse schrijven uit het klassediagram en testen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Checken of alle bestanden goed in github staan </t>
   </si>
   <si>
@@ -156,6 +144,12 @@
   </si>
   <si>
     <t xml:space="preserve">Onderzoeksrapport nakijken en klaar maken voor inleveren </t>
+  </si>
+  <si>
+    <t>Klasse schrijven</t>
+  </si>
+  <si>
+    <t>Doxygen documentatie nakijken</t>
   </si>
 </sst>
 </file>
@@ -832,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,15 +863,15 @@
       </c>
       <c r="J1" s="43"/>
       <c r="K1" s="29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>7</v>
@@ -914,17 +908,15 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="44"/>
       <c r="J3" s="45"/>
       <c r="K3" s="30">
+        <f>SUM(C3:J3)</f>
         <v>2</v>
       </c>
     </row>
@@ -933,21 +925,16 @@
       <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
       <c r="D4" s="7"/>
       <c r="E4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
       <c r="H4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="13">
-        <v>1.5</v>
+        <f>SUM(C4:J4)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -966,6 +953,7 @@
       <c r="H5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="13">
+        <f>SUM(C5:J5)</f>
         <v>2</v>
       </c>
     </row>
@@ -983,12 +971,10 @@
       </c>
       <c r="F6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="13">
-        <v>5</v>
+        <f>SUM(C6:J6)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -996,15 +982,25 @@
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="D7" s="7"/>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" s="7"/>
+      <c r="I7">
+        <v>1</v>
+      </c>
       <c r="J7" s="7"/>
       <c r="K7" s="13">
-        <v>3</v>
+        <f>SUM(C7:J7)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1012,116 +1008,123 @@
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
       <c r="D8" s="7"/>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="F8" s="7"/>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="13">
-        <v>2</v>
+        <f>SUM(C8:J8)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
+      <c r="B9" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9">
-        <v>1</v>
+      <c r="E9" s="15">
+        <v>10</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9">
-        <v>1</v>
+      <c r="G9" s="15">
+        <v>10</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="13">
-        <v>4</v>
+      <c r="I9" s="18">
+        <v>10</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="27">
+        <f>SUM(C9:J9)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1</v>
+      <c r="B10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10">
-        <v>1</v>
+      <c r="E10" s="17">
+        <v>10</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="15">
-        <v>1</v>
+      <c r="G10">
+        <v>10</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="13">
-        <v>4</v>
+        <f>SUM(C10:J10)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="7"/>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="13">
+        <f>SUM(C11:J11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="15">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="15">
-        <v>10</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="18">
-        <v>10</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="27">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
+      <c r="C12" s="17">
+        <v>2</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="13">
-        <v>40</v>
+        <f>SUM(C12:J12)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1129,17 +1132,25 @@
       <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="17">
+        <v>4</v>
+      </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="17">
+        <v>4</v>
+      </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="15">
-        <v>0.5</v>
+      <c r="G13">
+        <v>5</v>
       </c>
       <c r="H13" s="7"/>
+      <c r="I13">
+        <v>2</v>
+      </c>
       <c r="J13" s="7"/>
       <c r="K13" s="13">
-        <v>0.5</v>
+        <f>SUM(C13:J13)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1148,56 +1159,45 @@
         <v>20</v>
       </c>
       <c r="C14" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14">
-        <v>6</v>
-      </c>
       <c r="H14" s="7"/>
-      <c r="I14">
-        <v>2</v>
-      </c>
       <c r="J14" s="7"/>
       <c r="K14" s="13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <f>SUM(C14:J14)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
-      <c r="B15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="17">
-        <v>4</v>
-      </c>
+      <c r="B15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="17"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="17">
-        <v>4</v>
-      </c>
+      <c r="E15" s="17"/>
       <c r="F15" s="7"/>
-      <c r="G15">
-        <v>4</v>
-      </c>
       <c r="H15" s="7"/>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="13">
-        <v>16</v>
+        <f>SUM(C15:J15)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="17">
+      <c r="B16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="15">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="F16" s="7"/>
       <c r="G16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16">
@@ -1214,191 +1214,193 @@
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <f>SUM(C16:J16)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="17">
-        <v>2</v>
-      </c>
+      <c r="B17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="7"/>
-      <c r="G17">
-        <v>2</v>
-      </c>
       <c r="H17" s="7"/>
-      <c r="I17">
-        <v>2</v>
-      </c>
       <c r="J17" s="7"/>
       <c r="K17" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <f>SUM(C17:J17)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
-      <c r="B18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="15">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="17">
-        <v>2</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="22">
+        <f>SUM(C3:C17)</f>
+        <v>37.5</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22">
+        <f>SUM(E3:E17)</f>
+        <v>36</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22">
+        <f>SUM(G3:G17)</f>
+        <v>37</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22">
+        <f>SUM(I4:I17)</f>
+        <v>32</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="31">
+        <f>SUM(K3:K17)</f>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="43"/>
+      <c r="K19" s="25"/>
+    </row>
+    <row r="20" spans="1:12" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="26"/>
+      <c r="L20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19">
-        <v>1.5</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19">
-        <v>1.5</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="22">
-        <v>40</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22">
-        <v>41</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22">
-        <v>42</v>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22">
-        <v>35.5</v>
-      </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="31">
-        <v>161</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="25"/>
+      <c r="B21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="18">
+        <v>4</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="K21" s="27">
+        <f>SUM(C21:J21)</f>
+        <v>8</v>
+      </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K22" s="26"/>
+        <v>27</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="13">
+        <f>SUM(C22:J22)</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
-      <c r="B23" s="7" t="s">
-        <v>31</v>
+      <c r="B23" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F23" s="7"/>
+      <c r="G23">
+        <v>7</v>
+      </c>
       <c r="H23" s="7"/>
-      <c r="I23" s="18">
-        <v>4</v>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="27">
-        <v>8</v>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="13">
+        <f>SUM(C23:J23)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1407,427 +1409,411 @@
         <v>17</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <f>SUM(C24:J24)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
-        <v>40</v>
+      <c r="B25" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25">
-        <v>7</v>
-      </c>
       <c r="H25" s="7"/>
       <c r="I25">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="13">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <f>SUM(C25:J25)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
-      <c r="B26" s="7" t="s">
-        <v>20</v>
+      <c r="B26" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26">
-        <v>4</v>
-      </c>
       <c r="F26" s="7"/>
-      <c r="G26">
-        <v>4</v>
-      </c>
       <c r="H26" s="7"/>
       <c r="I26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <f>SUM(C26:J26)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="21">
+        <f>SUM(C21:C26)</f>
+        <v>27</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21">
+        <f>SUM(E21:E26)</f>
         <v>25</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="13">
+      <c r="F27" s="20"/>
+      <c r="G27" s="21">
+        <f>SUM(G21:G26)</f>
+        <v>21</v>
+      </c>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21">
+        <f>SUM(I21:I26)</f>
+        <v>31</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="28">
+        <f>SUM(K21:K26)</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="7"/>
+      <c r="E28">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="7"/>
       <c r="F28" s="7"/>
+      <c r="G28" s="15">
+        <v>3</v>
+      </c>
       <c r="H28" s="7"/>
+      <c r="I28">
+        <v>3</v>
+      </c>
       <c r="J28" s="7"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="13">
+        <f>SUM(C28:J28)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
-      <c r="B29" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="21">
-        <v>26</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21">
-        <v>24</v>
-      </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21">
-        <v>21</v>
-      </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21">
-        <v>26</v>
-      </c>
-      <c r="J29" s="20"/>
-      <c r="K29" s="28">
-        <v>94</v>
+      <c r="B29" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="17">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="27">
+        <f>SUM(C29:J29)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="15"/>
+      <c r="B30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="17">
+        <v>3</v>
+      </c>
       <c r="D30" s="7"/>
-      <c r="E30">
+      <c r="E30" s="17">
         <v>3</v>
       </c>
       <c r="F30" s="7"/>
-      <c r="G30" s="15">
+      <c r="G30" s="17">
         <v>3</v>
       </c>
       <c r="H30" s="7"/>
-      <c r="I30">
+      <c r="I30" s="32">
         <v>3</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="13">
-        <v>9</v>
+        <f>SUM(C30:J30)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
-      <c r="B31" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="17">
-        <v>3</v>
+      <c r="B31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="15">
+        <v>2</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="15">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="15">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H31" s="7"/>
-      <c r="I31" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="27">
-        <v>4.5</v>
+      <c r="I31" s="32">
+        <v>2</v>
+      </c>
+      <c r="J31" s="7"/>
+      <c r="K31" s="13">
+        <f>SUM(C31:J31)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C32" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F32" s="7"/>
-      <c r="G32" s="17">
-        <v>3</v>
-      </c>
       <c r="H32" s="7"/>
-      <c r="I32" s="32">
-        <v>3</v>
-      </c>
       <c r="J32" s="7"/>
       <c r="K32" s="13">
-        <v>12</v>
+        <f>SUM(C32:J32)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="15">
-        <v>2</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C33" s="15"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="15">
-        <v>2</v>
-      </c>
+      <c r="E33" s="15"/>
       <c r="F33" s="7"/>
       <c r="G33" s="15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H33" s="7"/>
-      <c r="I33" s="32">
-        <v>2</v>
+      <c r="I33">
+        <v>2.5</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="13">
-        <v>8</v>
+        <f>SUM(C33:J33)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
-      <c r="B34" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="17">
-        <v>1</v>
-      </c>
+      <c r="B34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="17"/>
       <c r="D34" s="7"/>
       <c r="E34" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F34" s="7"/>
+      <c r="G34" s="17">
+        <v>3</v>
+      </c>
       <c r="H34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <f>SUM(C34:J34)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
-      <c r="B35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="15"/>
+      <c r="B35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="17"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="15"/>
+      <c r="E35" s="17">
+        <v>2</v>
+      </c>
       <c r="F35" s="7"/>
-      <c r="G35" s="15">
-        <v>2.5</v>
+      <c r="G35" s="17">
+        <v>2</v>
       </c>
       <c r="H35" s="7"/>
-      <c r="I35">
-        <v>2.5</v>
-      </c>
       <c r="J35" s="7"/>
       <c r="K35" s="13">
-        <v>5</v>
+        <f>SUM(C35:J35)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="17">
-        <v>1</v>
+      <c r="B36" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="15">
+        <v>6</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <f>SUM(C36:J36)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="17">
-        <v>2</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="17">
-        <v>2</v>
-      </c>
+      <c r="C37" s="15">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="15"/>
       <c r="F37" s="7"/>
       <c r="G37" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" s="7"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
-      <c r="B38" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="15">
-        <v>6</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="17">
-        <v>6</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="17">
-        <v>6</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38">
-        <v>6</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="13">
+      <c r="B38" s="34" t="s">
         <v>24</v>
+      </c>
+      <c r="C38" s="35">
+        <f>SUM(C28:C37)</f>
+        <v>16</v>
+      </c>
+      <c r="D38" s="34"/>
+      <c r="E38" s="35">
+        <f>SUM(E28:E37)</f>
+        <v>20</v>
+      </c>
+      <c r="F38" s="34"/>
+      <c r="G38" s="35">
+        <f>SUM(G28:G37)</f>
+        <v>22.5</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="35">
+        <f>SUM(I28:I37)</f>
+        <v>17.5</v>
+      </c>
+      <c r="J38" s="33"/>
+      <c r="K38" s="31">
+        <v>70.5</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="13"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="33"/>
       <c r="B40" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="35">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C40" s="34">
+        <f>SUM(C38,C27,C18)</f>
+        <v>80.5</v>
       </c>
       <c r="D40" s="34"/>
-      <c r="E40" s="35">
-        <v>18.5</v>
+      <c r="E40" s="34">
+        <f>SUM(E38,E27,E18)</f>
+        <v>81</v>
       </c>
       <c r="F40" s="34"/>
-      <c r="G40" s="35">
-        <v>20</v>
+      <c r="G40" s="34">
+        <f>SUM(G38,G27,G18)</f>
+        <v>80.5</v>
       </c>
       <c r="H40" s="34"/>
-      <c r="I40" s="35">
-        <v>20</v>
-      </c>
-      <c r="J40" s="33"/>
-      <c r="K40" s="31">
-        <v>70.5</v>
+      <c r="I40" s="34">
+        <f>SUM(I38,I18,I27)</f>
+        <v>80.5</v>
+      </c>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34">
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="34"/>
-      <c r="B42" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="34">
-        <v>84</v>
-      </c>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34">
-        <v>83.5</v>
-      </c>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34">
-        <v>83</v>
-      </c>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34">
-        <v>81.5</v>
-      </c>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34">
-        <v>332</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
Object list and planning changed. Object list done
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Jip</t>
   </si>
@@ -107,9 +107,6 @@
     <t xml:space="preserve">Rik heeft hier minder uren omdat hij maandag en een deel van dinsdag er niet is </t>
   </si>
   <si>
-    <t>Week 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Onderzoek doen </t>
   </si>
   <si>
@@ -150,6 +147,15 @@
   </si>
   <si>
     <t>Doxygen documentatie nakijken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review momenten </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mijlpaal inleveren </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagelijks bestanden in gihub checken </t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +869,7 @@
       </c>
       <c r="J1" s="43"/>
       <c r="K1" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>25</v>
@@ -916,7 +922,7 @@
       <c r="I3" s="44"/>
       <c r="J3" s="45"/>
       <c r="K3" s="30">
-        <f>SUM(C3:J3)</f>
+        <f t="shared" ref="K3:K17" si="0">SUM(C3:J3)</f>
         <v>2</v>
       </c>
     </row>
@@ -933,7 +939,7 @@
       <c r="H4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="13">
-        <f>SUM(C4:J4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -953,7 +959,7 @@
       <c r="H5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="13">
-        <f>SUM(C5:J5)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -973,7 +979,7 @@
       <c r="H6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="13">
-        <f>SUM(C6:J6)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -999,7 +1005,7 @@
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="13">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1025,7 +1031,7 @@
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="13">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1051,14 +1057,14 @@
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="27">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1077,8 +1083,11 @@
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="13">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1097,8 +1106,11 @@
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="13">
-        <f>SUM(C11:J11)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1123,8 +1135,11 @@
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="13">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1149,7 +1164,7 @@
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="13">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -1169,7 +1184,7 @@
       <c r="H14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="13">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1188,7 +1203,7 @@
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="13">
-        <f>SUM(C15:J15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1214,7 +1229,7 @@
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="13">
-        <f>SUM(C16:J16)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1232,7 +1247,7 @@
       <c r="H17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="13">
-        <f>SUM(C17:J17)</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1324,11 +1339,9 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="A21" s="12"/>
       <c r="B21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1344,15 +1357,13 @@
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="27">
-        <f>SUM(C21:J21)</f>
+        <f t="shared" ref="K21:K26" si="1">SUM(C21:J21)</f>
         <v>8</v>
       </c>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="A22" s="9"/>
       <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
@@ -1373,14 +1384,14 @@
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="13">
-        <f>SUM(C22:J22)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -1399,7 +1410,7 @@
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="13">
-        <f>SUM(C23:J23)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -1425,7 +1436,7 @@
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="13">
-        <f>SUM(C24:J24)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1448,14 +1459,14 @@
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="13">
-        <f>SUM(C25:J25)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1468,7 +1479,7 @@
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="13">
-        <f>SUM(C26:J26)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1505,7 +1516,7 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="7"/>
@@ -1522,14 +1533,14 @@
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="13">
-        <f>SUM(C28:J28)</f>
+        <f t="shared" ref="K28:K36" si="2">SUM(C28:J28)</f>
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
       <c r="B29" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="17">
         <v>3</v>
@@ -1542,14 +1553,14 @@
       <c r="I29" s="18"/>
       <c r="J29" s="19"/>
       <c r="K29" s="27">
-        <f>SUM(C29:J29)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="17">
         <v>3</v>
@@ -1568,14 +1579,14 @@
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="13">
-        <f>SUM(C30:J30)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -1594,14 +1605,14 @@
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="13">
-        <f>SUM(C31:J31)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="17">
         <v>1</v>
@@ -1614,14 +1625,14 @@
       <c r="H32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="13">
-        <f>SUM(C32:J32)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="7"/>
@@ -1636,14 +1647,14 @@
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="13">
-        <f>SUM(C33:J33)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="7"/>
@@ -1657,14 +1668,14 @@
       <c r="H34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="13">
-        <f>SUM(C34:J34)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="7"/>
@@ -1678,14 +1689,14 @@
       <c r="H35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="13">
-        <f>SUM(C35:J35)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="15">
         <v>6</v>
@@ -1704,14 +1715,14 @@
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="13">
-        <f>SUM(C36:J36)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="15">
         <v>1</v>

</xml_diff>

<commit_message>
Added planning to final version
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\school\Desktop\the\Project_Laser_Turtle\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jip\Desktop\Project_Laser_Turtle\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9228"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -839,20 +839,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="39.140625" customWidth="1"/>
+    <col min="12" max="12" width="39.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -882,7 +882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="K2" s="26"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -935,26 +935,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>6</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" s="7">
-        <v>2</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="J4" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4</v>
+      </c>
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
       <c r="K4" s="13">
         <f>SUM(I4,G4,E4,C4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="7" t="s">
         <v>10</v>
@@ -981,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="7" t="s">
         <v>11</v>
@@ -990,22 +996,24 @@
         <v>2</v>
       </c>
       <c r="D6" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" s="7"/>
       <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
       <c r="K6" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="7" t="s">
         <v>12</v>
@@ -1020,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1037,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="7" t="s">
         <v>13</v>
@@ -1071,7 +1079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>15</v>
@@ -1079,25 +1087,33 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
       <c r="E9" s="15">
         <v>10</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
       <c r="G9" s="15">
         <v>10</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
       <c r="I9" s="18">
         <v>10</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="19">
+        <v>0</v>
+      </c>
       <c r="K9" s="13">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>39</v>
@@ -1105,7 +1121,9 @@
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
       <c r="E10" s="17">
         <v>10</v>
       </c>
@@ -1120,7 +1138,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="0"/>
@@ -1130,15 +1148,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
       <c r="G11" s="15"/>
       <c r="H11" s="7"/>
       <c r="I11">
@@ -1153,7 +1175,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="7" t="s">
         <v>17</v>
@@ -1165,15 +1187,21 @@
       <c r="E12" s="17">
         <v>2</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12">
         <v>6</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
       <c r="I12">
         <v>3</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
       <c r="K12" s="13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1182,7 +1210,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="7" t="s">
         <v>19</v>
@@ -1196,7 +1224,9 @@
       <c r="E13" s="17">
         <v>4</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
       <c r="G13">
         <v>5</v>
       </c>
@@ -1206,13 +1236,15 @@
       <c r="I13">
         <v>2</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7">
+        <v>4</v>
+      </c>
       <c r="K13" s="13">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="7" t="s">
         <v>20</v>
@@ -1240,7 +1272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>21</v>
@@ -1255,13 +1287,15 @@
       <c r="I15">
         <v>2</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
       <c r="K15" s="13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="16" t="s">
         <v>22</v>
@@ -1269,25 +1303,33 @@
       <c r="C16" s="15">
         <v>1</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
       <c r="E16" s="17">
         <v>1</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
       <c r="G16">
         <v>4</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7">
+        <v>6</v>
+      </c>
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="7">
+        <v>3</v>
+      </c>
       <c r="K16" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="16" t="s">
         <v>23</v>
@@ -1295,7 +1337,9 @@
       <c r="C17" s="15">
         <v>1.5</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="16">
+        <v>3</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="7"/>
       <c r="H17" s="7"/>
@@ -1305,7 +1349,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>42670</v>
       </c>
@@ -1322,7 +1366,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="41"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="21" t="s">
         <v>24</v>
@@ -1333,7 +1377,7 @@
       </c>
       <c r="D19" s="21">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" si="1"/>
@@ -1341,7 +1385,7 @@
       </c>
       <c r="F19" s="21">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="1"/>
@@ -1349,7 +1393,7 @@
       </c>
       <c r="H19" s="21">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I19" s="22">
         <f>SUM(I4:I17)</f>
@@ -1357,14 +1401,14 @@
       </c>
       <c r="J19" s="20">
         <f>SUM(J4:J17)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K19" s="13">
         <f>SUM(I19,G19,E19,C19)</f>
         <v>142.5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>7</v>
@@ -1387,7 +1431,7 @@
       <c r="J20" s="51"/>
       <c r="K20" s="25"/>
     </row>
-    <row r="21" spans="1:12" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20"/>
       <c r="B21" s="8" t="s">
         <v>7</v>
@@ -1421,7 +1465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="7" t="s">
         <v>27</v>
@@ -1429,25 +1473,31 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
       <c r="E22">
         <v>2</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
       <c r="H22" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I22" s="18">
         <v>4</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="19">
+        <v>2</v>
+      </c>
       <c r="K22" s="27">
         <f>SUM(I22,E22,C22,G22)</f>
         <v>8</v>
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="7" t="s">
         <v>15</v>
@@ -1455,25 +1505,33 @@
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
       <c r="E23">
         <v>10</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>10</v>
+      </c>
       <c r="G23">
         <v>10</v>
       </c>
-      <c r="H23" s="7"/>
+      <c r="H23" s="7">
+        <v>0</v>
+      </c>
       <c r="I23">
         <v>10</v>
       </c>
-      <c r="J23" s="7"/>
+      <c r="J23" s="7">
+        <v>0</v>
+      </c>
       <c r="K23" s="27">
         <f t="shared" ref="K23:K40" si="2">SUM(I23,E23,C23,G23)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>39</v>
@@ -1481,25 +1539,33 @@
       <c r="C24">
         <v>7</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7">
+        <v>7</v>
+      </c>
       <c r="E24">
         <v>7</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>4</v>
+      </c>
       <c r="G24">
         <v>7</v>
       </c>
-      <c r="H24" s="7"/>
+      <c r="H24" s="7">
+        <v>6</v>
+      </c>
       <c r="I24">
         <v>9</v>
       </c>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7">
+        <v>16</v>
+      </c>
       <c r="K24" s="27">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="7" t="s">
         <v>17</v>
@@ -1507,25 +1573,33 @@
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>2</v>
+      </c>
       <c r="E25">
         <v>4</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>4</v>
+      </c>
       <c r="G25">
         <v>4</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="7">
+        <v>2</v>
+      </c>
       <c r="I25">
         <v>4</v>
       </c>
-      <c r="J25" s="7"/>
+      <c r="J25" s="7">
+        <v>2</v>
+      </c>
       <c r="K25" s="27">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
         <v>22</v>
@@ -1534,7 +1608,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1543,20 +1617,20 @@
         <v>1.5</v>
       </c>
       <c r="H26" s="7">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I26">
         <v>2</v>
       </c>
       <c r="J26" s="7">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="K26" s="27">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>38</v>
@@ -1572,13 +1646,15 @@
       <c r="I27">
         <v>2</v>
       </c>
-      <c r="J27" s="7"/>
+      <c r="J27" s="7">
+        <v>0.5</v>
+      </c>
       <c r="K27" s="27">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>42675</v>
       </c>
@@ -1595,7 +1671,7 @@
       <c r="J28" s="40"/>
       <c r="K28" s="43"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10"/>
       <c r="B29" s="20" t="s">
         <v>24</v>
@@ -1606,7 +1682,7 @@
       </c>
       <c r="D29" s="20">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>19.5</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
@@ -1614,7 +1690,7 @@
       </c>
       <c r="F29" s="20">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>21.5</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="3"/>
@@ -1622,7 +1698,7 @@
       </c>
       <c r="H29" s="20">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" si="3"/>
@@ -1630,14 +1706,14 @@
       </c>
       <c r="J29" s="20">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>26.5</v>
       </c>
       <c r="K29" s="27">
         <f>SUM(I29,E29,C29,G29)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
         <v>29</v>
@@ -1669,7 +1745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
       <c r="B31" s="11" t="s">
         <v>30</v>
@@ -1677,19 +1753,23 @@
       <c r="C31" s="17">
         <v>3</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="7">
+        <v>3</v>
+      </c>
       <c r="E31" s="15"/>
       <c r="F31" s="7"/>
       <c r="G31" s="15"/>
       <c r="H31" s="7"/>
       <c r="I31" s="18"/>
-      <c r="J31" s="19"/>
+      <c r="J31" s="19">
+        <v>2</v>
+      </c>
       <c r="K31" s="27">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>33</v>
@@ -1697,25 +1777,33 @@
       <c r="C32" s="17">
         <v>3</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7">
+        <v>0</v>
+      </c>
       <c r="E32" s="17">
         <v>3</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
       <c r="G32" s="17">
         <v>3</v>
       </c>
-      <c r="H32" s="7"/>
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
       <c r="I32" s="30">
         <v>3</v>
       </c>
-      <c r="J32" s="7"/>
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
       <c r="K32" s="27">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="7" t="s">
         <v>34</v>
@@ -1723,25 +1811,33 @@
       <c r="C33" s="15">
         <v>2</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7">
+        <v>4</v>
+      </c>
       <c r="E33" s="15">
         <v>2</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
       <c r="G33" s="15">
         <v>2</v>
       </c>
-      <c r="H33" s="7"/>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
       <c r="I33" s="30">
         <v>2</v>
       </c>
-      <c r="J33" s="7"/>
+      <c r="J33" s="7">
+        <v>1</v>
+      </c>
       <c r="K33" s="27">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11" t="s">
         <v>31</v>
@@ -1749,11 +1845,15 @@
       <c r="C34" s="17">
         <v>1</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
       <c r="E34" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
       <c r="H34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="27">
@@ -1761,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
         <v>32</v>
@@ -1773,17 +1873,21 @@
       <c r="G35" s="15">
         <v>2.5</v>
       </c>
-      <c r="H35" s="7"/>
+      <c r="H35" s="7">
+        <v>2.5</v>
+      </c>
       <c r="I35">
         <v>2.5</v>
       </c>
-      <c r="J35" s="7"/>
+      <c r="J35" s="7">
+        <v>2.5</v>
+      </c>
       <c r="K35" s="27">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
         <v>35</v>
@@ -1793,39 +1897,49 @@
       <c r="E36" s="17">
         <v>3</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7">
+        <v>2</v>
+      </c>
       <c r="G36" s="17">
         <v>3</v>
       </c>
-      <c r="H36" s="7"/>
+      <c r="H36" s="7">
+        <v>2</v>
+      </c>
       <c r="J36" s="7"/>
       <c r="K36" s="27">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="7"/>
+      <c r="D37" s="7">
+        <v>2</v>
+      </c>
       <c r="E37" s="17">
         <v>2</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
       <c r="G37" s="17">
         <v>2</v>
       </c>
-      <c r="H37" s="7"/>
+      <c r="H37" s="7">
+        <v>0</v>
+      </c>
       <c r="J37" s="7"/>
       <c r="K37" s="27">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="16" t="s">
         <v>37</v>
@@ -1833,25 +1947,33 @@
       <c r="C38" s="15">
         <v>6</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="7">
+        <v>16</v>
+      </c>
       <c r="E38" s="17">
         <v>6</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7">
+        <v>16</v>
+      </c>
       <c r="G38" s="17">
         <v>6</v>
       </c>
-      <c r="H38" s="7"/>
+      <c r="H38" s="7">
+        <v>6</v>
+      </c>
       <c r="I38">
         <v>6</v>
       </c>
-      <c r="J38" s="7"/>
+      <c r="J38" s="7">
+        <v>10</v>
+      </c>
       <c r="K38" s="27">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="16" t="s">
         <v>45</v>
@@ -1883,7 +2005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="32" t="s">
         <v>24</v>
@@ -1894,7 +2016,7 @@
       </c>
       <c r="D40" s="32">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E40" s="33">
         <f t="shared" si="4"/>
@@ -1902,7 +2024,7 @@
       </c>
       <c r="F40" s="32">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G40" s="33">
         <f t="shared" si="4"/>
@@ -1910,7 +2032,7 @@
       </c>
       <c r="H40" s="32">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>20.5</v>
       </c>
       <c r="I40" s="33">
         <f t="shared" si="4"/>
@@ -1918,14 +2040,14 @@
       </c>
       <c r="J40" s="31">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>23.5</v>
       </c>
       <c r="K40" s="27">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1938,7 +2060,7 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="31"/>
       <c r="B42" s="32" t="s">
         <v>14</v>
@@ -1947,30 +2069,42 @@
         <f>SUM(C40,C29,C19)</f>
         <v>80.5</v>
       </c>
-      <c r="D42" s="32"/>
+      <c r="D42" s="32">
+        <f>SUM(D40,D29,D19)</f>
+        <v>89.5</v>
+      </c>
       <c r="E42" s="32">
         <f>SUM(E40,E29,E19)</f>
         <v>81</v>
       </c>
-      <c r="F42" s="32"/>
+      <c r="F42" s="32">
+        <f>SUM(F29,F40,F19)</f>
+        <v>83.5</v>
+      </c>
       <c r="G42" s="32">
         <f>SUM(G40,G29,G19)</f>
         <v>80.5</v>
       </c>
-      <c r="H42" s="32"/>
+      <c r="H42" s="32">
+        <f>SUM(H40,H29,H19)</f>
+        <v>81.5</v>
+      </c>
       <c r="I42" s="32">
         <f>SUM(I40,I19,I29)</f>
         <v>80.5</v>
       </c>
-      <c r="J42" s="32"/>
+      <c r="J42" s="32">
+        <f>SUM(J40,J29,J19)</f>
+        <v>80</v>
+      </c>
       <c r="K42" s="32">
         <v>332</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="32"/>
     </row>
   </sheetData>

</xml_diff>